<commit_message>
Looking at serial monitor data to compare std dev to matlab data
</commit_message>
<xml_diff>
--- a/AL20v1_2024-04-11/Serial monitor baud 9600.xlsx
+++ b/AL20v1_2024-04-11/Serial monitor baud 9600.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smartin/Documents/MATLAB/GitHub/windtunnel/AL20v1_2024-04-11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samjkmartin/Documents/MATLAB/windtunnel/AL20v1_2024-04-11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A82F01-2477-524A-9519-D4312DA8CAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22848A1-8E41-104B-AAAC-9AFAD7BB4235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15920" xr2:uid="{D0CE5EC4-32EF-814C-98EC-99D7FD143F4E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1916" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1917" uniqueCount="346">
   <si>
     <t>18:04:18.797</t>
   </si>
@@ -1071,6 +1071,9 @@
   </si>
   <si>
     <t>Voltage</t>
+  </si>
+  <si>
+    <t>160 Hz</t>
   </si>
 </sst>
 </file>
@@ -13795,10 +13798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD4DB7F-D5D6-8B43-975D-11B29EFCC394}">
-  <dimension ref="A1:B1915"/>
+  <dimension ref="A1:C1915"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13806,15 +13809,18 @@
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>343</v>
       </c>
       <c r="B1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -13822,7 +13828,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -13830,7 +13836,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -13838,7 +13844,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -13846,7 +13852,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -13854,7 +13860,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -13862,7 +13868,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -13870,7 +13876,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -13878,7 +13884,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -13886,7 +13892,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -13894,7 +13900,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -13902,7 +13908,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -13910,7 +13916,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -13918,7 +13924,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -13926,7 +13932,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>